<commit_message>
process operations as list, 0.5 of finance app converted, feb budget reviewed
</commit_message>
<xml_diff>
--- a/backups/transactions.xlsx
+++ b/backups/transactions.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1237"/>
+  <dimension ref="A1:N1246"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -66039,6 +66039,452 @@
       </c>
       <c r="M1237" t="inlineStr"/>
       <c r="N1237" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" s="1" t="inlineStr">
+        <is>
+          <t>a19bd1c9-1ebf-473c-a43f-f386de448571</t>
+        </is>
+      </c>
+      <c r="B1238" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1238" t="inlineStr"/>
+      <c r="D1238" s="2" t="n">
+        <v>44975</v>
+      </c>
+      <c r="E1238" s="2" t="n">
+        <v>44976</v>
+      </c>
+      <c r="F1238" t="inlineStr">
+        <is>
+          <t>ALL HEART YOGA</t>
+        </is>
+      </c>
+      <c r="G1238" t="inlineStr">
+        <is>
+          <t>Personal</t>
+        </is>
+      </c>
+      <c r="H1238" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1238" t="n">
+        <v>-128</v>
+      </c>
+      <c r="J1238" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1238" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1238" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1238" t="inlineStr"/>
+      <c r="N1238" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" s="1" t="inlineStr">
+        <is>
+          <t>20ccf7d9-2bf2-4951-8527-c6fdba0d191e</t>
+        </is>
+      </c>
+      <c r="B1239" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1239" t="inlineStr"/>
+      <c r="D1239" s="2" t="n">
+        <v>44974</v>
+      </c>
+      <c r="E1239" s="2" t="n">
+        <v>44976</v>
+      </c>
+      <c r="F1239" t="inlineStr">
+        <is>
+          <t>REI.COM  800-426-4840</t>
+        </is>
+      </c>
+      <c r="G1239" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="H1239" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1239" t="n">
+        <v>-83.09</v>
+      </c>
+      <c r="J1239" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1239" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1239" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1239" t="inlineStr"/>
+      <c r="N1239" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" s="1" t="inlineStr">
+        <is>
+          <t>72947e24-823d-4c64-aa9b-e877cce88df1</t>
+        </is>
+      </c>
+      <c r="B1240" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1240" t="inlineStr"/>
+      <c r="D1240" s="2" t="n">
+        <v>44974</v>
+      </c>
+      <c r="E1240" s="2" t="n">
+        <v>44974</v>
+      </c>
+      <c r="F1240" t="inlineStr">
+        <is>
+          <t>GRAMMARLY COMVZBK3Q</t>
+        </is>
+      </c>
+      <c r="G1240" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="H1240" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1240" t="n">
+        <v>-86.40000000000001</v>
+      </c>
+      <c r="J1240" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1240" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1240" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1240" t="inlineStr"/>
+      <c r="N1240" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" s="1" t="inlineStr">
+        <is>
+          <t>e3b1ff1b-cfe5-448e-b91f-8c5fed83a3fa</t>
+        </is>
+      </c>
+      <c r="B1241" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1241" t="inlineStr"/>
+      <c r="D1241" s="2" t="n">
+        <v>44971</v>
+      </c>
+      <c r="E1241" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="F1241" t="inlineStr">
+        <is>
+          <t>SQ *JD'S SHOE REPAIR</t>
+        </is>
+      </c>
+      <c r="G1241" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="H1241" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1241" t="n">
+        <v>-100</v>
+      </c>
+      <c r="J1241" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1241" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1241" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1241" t="inlineStr"/>
+      <c r="N1241" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" s="1" t="inlineStr">
+        <is>
+          <t>be0653d1-18c8-47c4-ad5e-37ff893f5298</t>
+        </is>
+      </c>
+      <c r="B1242" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1242" t="inlineStr"/>
+      <c r="D1242" s="2" t="n">
+        <v>44971</v>
+      </c>
+      <c r="E1242" s="2" t="n">
+        <v>44972</v>
+      </c>
+      <c r="F1242" t="inlineStr">
+        <is>
+          <t>76 - PLAID PANTRY 83</t>
+        </is>
+      </c>
+      <c r="G1242" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="H1242" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1242" t="n">
+        <v>-34.01</v>
+      </c>
+      <c r="J1242" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1242" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1242" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1242" t="inlineStr"/>
+      <c r="N1242" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" s="1" t="inlineStr">
+        <is>
+          <t>1f7db794-5f46-40d5-88b9-236d8dbc6d1e</t>
+        </is>
+      </c>
+      <c r="B1243" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1243" t="inlineStr"/>
+      <c r="D1243" s="2" t="n">
+        <v>44976</v>
+      </c>
+      <c r="E1243" s="2" t="n">
+        <v>44977</v>
+      </c>
+      <c r="F1243" t="inlineStr">
+        <is>
+          <t>SQ *BARISTA</t>
+        </is>
+      </c>
+      <c r="G1243" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1243" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1243" t="n">
+        <v>-12.75</v>
+      </c>
+      <c r="J1243" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1243" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1243" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1243" t="inlineStr"/>
+      <c r="N1243" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" s="1" t="inlineStr">
+        <is>
+          <t>df528fc9-13a1-4819-bb69-a51b760d0852</t>
+        </is>
+      </c>
+      <c r="B1244" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1244" t="inlineStr"/>
+      <c r="D1244" s="2" t="n">
+        <v>44976</v>
+      </c>
+      <c r="E1244" s="2" t="n">
+        <v>44977</v>
+      </c>
+      <c r="F1244" t="inlineStr">
+        <is>
+          <t>SQ *CLEARING CAFE</t>
+        </is>
+      </c>
+      <c r="G1244" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1244" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1244" t="n">
+        <v>-6.5</v>
+      </c>
+      <c r="J1244" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1244" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1244" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1244" t="inlineStr"/>
+      <c r="N1244" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" s="1" t="inlineStr">
+        <is>
+          <t>35ea6bfe-112b-46e4-b63c-dfac5ccb7d6e</t>
+        </is>
+      </c>
+      <c r="B1245" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1245" t="inlineStr"/>
+      <c r="D1245" s="2" t="n">
+        <v>44975</v>
+      </c>
+      <c r="E1245" s="2" t="n">
+        <v>44976</v>
+      </c>
+      <c r="F1245" t="inlineStr">
+        <is>
+          <t>SQ *BARISTA</t>
+        </is>
+      </c>
+      <c r="G1245" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1245" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1245" t="n">
+        <v>-7.75</v>
+      </c>
+      <c r="J1245" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1245" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1245" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1245" t="inlineStr"/>
+      <c r="N1245" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" s="1" t="inlineStr">
+        <is>
+          <t>e9742163-c168-4601-b329-c0a1e9f351f9</t>
+        </is>
+      </c>
+      <c r="B1246" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="C1246" t="inlineStr"/>
+      <c r="D1246" s="2" t="n">
+        <v>44974</v>
+      </c>
+      <c r="E1246" s="2" t="n">
+        <v>44974</v>
+      </c>
+      <c r="F1246" t="inlineStr">
+        <is>
+          <t>AUTOMATIC PAYMENT - THANK</t>
+        </is>
+      </c>
+      <c r="G1246" t="inlineStr"/>
+      <c r="H1246" t="inlineStr">
+        <is>
+          <t>Payment</t>
+        </is>
+      </c>
+      <c r="I1246" t="n">
+        <v>1074.39</v>
+      </c>
+      <c r="J1246" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="K1246" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1246" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1246" t="inlineStr"/>
+      <c r="N1246" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Taxes app update and start
</commit_message>
<xml_diff>
--- a/backups/transactions.xlsx
+++ b/backups/transactions.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1246"/>
+  <dimension ref="A1:N1266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -64688,7 +64688,7 @@
         <v>44970</v>
       </c>
       <c r="C1213" s="2" t="n">
-        <v>44970</v>
+        <v>44990</v>
       </c>
       <c r="D1213" s="2" t="n">
         <v>44966</v>
@@ -64727,7 +64727,7 @@
       </c>
       <c r="M1213" t="inlineStr">
         <is>
-          <t>Eating Out</t>
+          <t>Haircut</t>
         </is>
       </c>
       <c r="N1213" t="n">
@@ -66051,7 +66051,9 @@
       <c r="B1238" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1238" t="inlineStr"/>
+      <c r="C1238" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1238" s="2" t="n">
         <v>44975</v>
       </c>
@@ -66085,9 +66087,13 @@
         </is>
       </c>
       <c r="L1238" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1238" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1238" t="inlineStr">
+        <is>
+          <t>Yoga</t>
+        </is>
+      </c>
       <c r="N1238" t="n">
         <v>0</v>
       </c>
@@ -66101,7 +66107,9 @@
       <c r="B1239" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1239" t="inlineStr"/>
+      <c r="C1239" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1239" s="2" t="n">
         <v>44974</v>
       </c>
@@ -66135,9 +66143,13 @@
         </is>
       </c>
       <c r="L1239" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1239" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1239" t="inlineStr">
+        <is>
+          <t>Gifts</t>
+        </is>
+      </c>
       <c r="N1239" t="n">
         <v>0</v>
       </c>
@@ -66151,7 +66163,9 @@
       <c r="B1240" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1240" t="inlineStr"/>
+      <c r="C1240" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1240" s="2" t="n">
         <v>44974</v>
       </c>
@@ -66185,9 +66199,13 @@
         </is>
       </c>
       <c r="L1240" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1240" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1240" t="inlineStr">
+        <is>
+          <t>Services</t>
+        </is>
+      </c>
       <c r="N1240" t="n">
         <v>0</v>
       </c>
@@ -66201,7 +66219,9 @@
       <c r="B1241" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1241" t="inlineStr"/>
+      <c r="C1241" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1241" s="2" t="n">
         <v>44971</v>
       </c>
@@ -66235,9 +66255,13 @@
         </is>
       </c>
       <c r="L1241" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1241" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1241" t="inlineStr">
+        <is>
+          <t>Clothes</t>
+        </is>
+      </c>
       <c r="N1241" t="n">
         <v>0</v>
       </c>
@@ -66251,7 +66275,9 @@
       <c r="B1242" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1242" t="inlineStr"/>
+      <c r="C1242" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1242" s="2" t="n">
         <v>44971</v>
       </c>
@@ -66285,9 +66311,13 @@
         </is>
       </c>
       <c r="L1242" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1242" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1242" t="inlineStr">
+        <is>
+          <t>Gasoline</t>
+        </is>
+      </c>
       <c r="N1242" t="n">
         <v>0</v>
       </c>
@@ -66301,7 +66331,9 @@
       <c r="B1243" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1243" t="inlineStr"/>
+      <c r="C1243" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1243" s="2" t="n">
         <v>44976</v>
       </c>
@@ -66335,9 +66367,13 @@
         </is>
       </c>
       <c r="L1243" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1243" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1243" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
       <c r="N1243" t="n">
         <v>0</v>
       </c>
@@ -66351,7 +66387,9 @@
       <c r="B1244" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1244" t="inlineStr"/>
+      <c r="C1244" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1244" s="2" t="n">
         <v>44976</v>
       </c>
@@ -66385,9 +66423,13 @@
         </is>
       </c>
       <c r="L1244" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1244" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1244" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
       <c r="N1244" t="n">
         <v>0</v>
       </c>
@@ -66401,7 +66443,9 @@
       <c r="B1245" s="2" t="n">
         <v>44984</v>
       </c>
-      <c r="C1245" t="inlineStr"/>
+      <c r="C1245" s="2" t="n">
+        <v>44989</v>
+      </c>
       <c r="D1245" s="2" t="n">
         <v>44975</v>
       </c>
@@ -66435,9 +66479,13 @@
         </is>
       </c>
       <c r="L1245" t="n">
-        <v>0</v>
-      </c>
-      <c r="M1245" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="M1245" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
       <c r="N1245" t="n">
         <v>0</v>
       </c>
@@ -66485,6 +66533,1090 @@
       </c>
       <c r="M1246" t="inlineStr"/>
       <c r="N1246" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" s="1" t="inlineStr">
+        <is>
+          <t>8c0d1dde-135e-4134-9d2e-197454e5e632</t>
+        </is>
+      </c>
+      <c r="B1247" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1247" t="inlineStr"/>
+      <c r="D1247" s="2" t="n">
+        <v>44985</v>
+      </c>
+      <c r="E1247" s="2" t="n">
+        <v>44985</v>
+      </c>
+      <c r="F1247" t="inlineStr">
+        <is>
+          <t>AUTOMATIC PAYMENT - THANK</t>
+        </is>
+      </c>
+      <c r="G1247" t="inlineStr"/>
+      <c r="H1247" t="inlineStr">
+        <is>
+          <t>Payment</t>
+        </is>
+      </c>
+      <c r="I1247" t="n">
+        <v>2186.84</v>
+      </c>
+      <c r="J1247" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1247" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1247" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1247" t="inlineStr"/>
+      <c r="N1247" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" s="1" t="inlineStr">
+        <is>
+          <t>0df3bdec-4e8d-4085-b6e1-e49b33650ce0</t>
+        </is>
+      </c>
+      <c r="B1248" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1248" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1248" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="E1248" s="2" t="n">
+        <v>44985</v>
+      </c>
+      <c r="F1248" t="inlineStr">
+        <is>
+          <t>CVS/PHARMACY #06920</t>
+        </is>
+      </c>
+      <c r="G1248" t="inlineStr">
+        <is>
+          <t>Health &amp; Wellness</t>
+        </is>
+      </c>
+      <c r="H1248" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1248" t="n">
+        <v>-27.15</v>
+      </c>
+      <c r="J1248" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1248" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1248" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1248" t="inlineStr">
+        <is>
+          <t>Services</t>
+        </is>
+      </c>
+      <c r="N1248" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" s="1" t="inlineStr">
+        <is>
+          <t>c1b247ae-7d33-4265-9933-3b89419fabd9</t>
+        </is>
+      </c>
+      <c r="B1249" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1249" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1249" s="2" t="n">
+        <v>44982</v>
+      </c>
+      <c r="E1249" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="F1249" t="inlineStr">
+        <is>
+          <t>PEARL HARDWARE</t>
+        </is>
+      </c>
+      <c r="G1249" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="H1249" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1249" t="n">
+        <v>-1.14</v>
+      </c>
+      <c r="J1249" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1249" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1249" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1249" t="inlineStr">
+        <is>
+          <t>Jeep</t>
+        </is>
+      </c>
+      <c r="N1249" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" s="1" t="inlineStr">
+        <is>
+          <t>12a23086-9297-496e-bce7-55fca1a5d5c9</t>
+        </is>
+      </c>
+      <c r="B1250" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1250" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1250" s="2" t="n">
+        <v>44982</v>
+      </c>
+      <c r="E1250" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="F1250" t="inlineStr">
+        <is>
+          <t>CITY OF PORTLAND DEPT</t>
+        </is>
+      </c>
+      <c r="G1250" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="H1250" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1250" t="n">
+        <v>-2.2</v>
+      </c>
+      <c r="J1250" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1250" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1250" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1250" t="inlineStr">
+        <is>
+          <t>Parking</t>
+        </is>
+      </c>
+      <c r="N1250" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" s="1" t="inlineStr">
+        <is>
+          <t>dcd8495c-bb33-484e-9b02-eba300650966</t>
+        </is>
+      </c>
+      <c r="B1251" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1251" s="2" t="n">
+        <v>44990</v>
+      </c>
+      <c r="D1251" s="2" t="n">
+        <v>44981</v>
+      </c>
+      <c r="E1251" s="2" t="n">
+        <v>44981</v>
+      </c>
+      <c r="F1251" t="inlineStr">
+        <is>
+          <t>COMCAST CABLE COMM</t>
+        </is>
+      </c>
+      <c r="G1251" t="inlineStr">
+        <is>
+          <t>Bills &amp; Utilities</t>
+        </is>
+      </c>
+      <c r="H1251" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1251" t="n">
+        <v>-44.99</v>
+      </c>
+      <c r="J1251" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1251" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1251" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1251" t="inlineStr">
+        <is>
+          <t>Internet</t>
+        </is>
+      </c>
+      <c r="N1251" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" s="1" t="inlineStr">
+        <is>
+          <t>abab1a3d-397b-4af0-8c1d-1c7193930558</t>
+        </is>
+      </c>
+      <c r="B1252" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1252" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1252" s="2" t="n">
+        <v>44978</v>
+      </c>
+      <c r="E1252" s="2" t="n">
+        <v>44979</v>
+      </c>
+      <c r="F1252" t="inlineStr">
+        <is>
+          <t>GOOGLE *Domains</t>
+        </is>
+      </c>
+      <c r="G1252" t="inlineStr">
+        <is>
+          <t>Personal</t>
+        </is>
+      </c>
+      <c r="H1252" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1252" t="n">
+        <v>-6</v>
+      </c>
+      <c r="J1252" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1252" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="L1252" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1252" t="inlineStr">
+        <is>
+          <t>Services</t>
+        </is>
+      </c>
+      <c r="N1252" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" s="1" t="inlineStr">
+        <is>
+          <t>8d87ca6f-37f1-47f3-a97a-83b7a959341e</t>
+        </is>
+      </c>
+      <c r="B1253" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1253" s="2" t="n">
+        <v>44990</v>
+      </c>
+      <c r="D1253" s="2" t="n">
+        <v>44985</v>
+      </c>
+      <c r="E1253" s="2" t="n">
+        <v>44986</v>
+      </c>
+      <c r="F1253" t="inlineStr">
+        <is>
+          <t>THE FRISCO BAR &amp;amp; GRILL</t>
+        </is>
+      </c>
+      <c r="G1253" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1253" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1253" t="n">
+        <v>-36.88</v>
+      </c>
+      <c r="J1253" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1253" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1253" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1253" t="inlineStr">
+        <is>
+          <t>Entertainment</t>
+        </is>
+      </c>
+      <c r="N1253" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" s="1" t="inlineStr">
+        <is>
+          <t>f5e60baf-78cd-4d7e-8828-3babdc7f617f</t>
+        </is>
+      </c>
+      <c r="B1254" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1254" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1254" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="E1254" s="2" t="n">
+        <v>44985</v>
+      </c>
+      <c r="F1254" t="inlineStr">
+        <is>
+          <t>ANGELINAS RESTAURANT</t>
+        </is>
+      </c>
+      <c r="G1254" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1254" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1254" t="n">
+        <v>-37.92</v>
+      </c>
+      <c r="J1254" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1254" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1254" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1254" t="inlineStr">
+        <is>
+          <t>Travel</t>
+        </is>
+      </c>
+      <c r="N1254" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" s="1" t="inlineStr">
+        <is>
+          <t>026cc162-e9dc-4c81-89cd-a57b600f11a1</t>
+        </is>
+      </c>
+      <c r="B1255" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1255" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1255" s="2" t="n">
+        <v>44983</v>
+      </c>
+      <c r="E1255" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="F1255" t="inlineStr">
+        <is>
+          <t>SQ *UPPER LEFT ROASTERS</t>
+        </is>
+      </c>
+      <c r="G1255" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1255" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1255" t="n">
+        <v>-5.25</v>
+      </c>
+      <c r="J1255" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1255" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1255" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1255" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="N1255" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" s="1" t="inlineStr">
+        <is>
+          <t>e513dd92-7424-4a7a-868f-ea8106b5ffbc</t>
+        </is>
+      </c>
+      <c r="B1256" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1256" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1256" s="2" t="n">
+        <v>44983</v>
+      </c>
+      <c r="E1256" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="F1256" t="inlineStr">
+        <is>
+          <t>BAR WEST</t>
+        </is>
+      </c>
+      <c r="G1256" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1256" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1256" t="n">
+        <v>-40</v>
+      </c>
+      <c r="J1256" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1256" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1256" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1256" t="inlineStr">
+        <is>
+          <t>Eating Out</t>
+        </is>
+      </c>
+      <c r="N1256" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" s="1" t="inlineStr">
+        <is>
+          <t>02862eca-c48c-442f-a48e-0f4a573f9693</t>
+        </is>
+      </c>
+      <c r="B1257" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1257" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1257" s="2" t="n">
+        <v>44983</v>
+      </c>
+      <c r="E1257" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="F1257" t="inlineStr">
+        <is>
+          <t>SQ *UPPER LEFT ROASTERS</t>
+        </is>
+      </c>
+      <c r="G1257" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1257" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1257" t="n">
+        <v>-21.3</v>
+      </c>
+      <c r="J1257" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1257" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1257" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1257" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="N1257" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" s="1" t="inlineStr">
+        <is>
+          <t>c9c122bf-7090-44aa-9e46-9c4cb019fd81</t>
+        </is>
+      </c>
+      <c r="B1258" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1258" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1258" s="2" t="n">
+        <v>44982</v>
+      </c>
+      <c r="E1258" s="2" t="n">
+        <v>44984</v>
+      </c>
+      <c r="F1258" t="inlineStr">
+        <is>
+          <t>ARCO#83189GURU NANAK 13</t>
+        </is>
+      </c>
+      <c r="G1258" t="inlineStr">
+        <is>
+          <t>Gas</t>
+        </is>
+      </c>
+      <c r="H1258" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1258" t="n">
+        <v>-42.81</v>
+      </c>
+      <c r="J1258" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1258" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1258" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1258" t="inlineStr">
+        <is>
+          <t>Gasoline</t>
+        </is>
+      </c>
+      <c r="N1258" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" s="1" t="inlineStr">
+        <is>
+          <t>4f504a92-096d-423c-ba4e-d79a1e8d83b4</t>
+        </is>
+      </c>
+      <c r="B1259" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1259" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1259" s="2" t="n">
+        <v>44980</v>
+      </c>
+      <c r="E1259" s="2" t="n">
+        <v>44983</v>
+      </c>
+      <c r="F1259" t="inlineStr">
+        <is>
+          <t>SAINT HONORE BOULANGERIE</t>
+        </is>
+      </c>
+      <c r="G1259" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1259" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1259" t="n">
+        <v>-12.6</v>
+      </c>
+      <c r="J1259" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1259" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1259" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1259" t="inlineStr">
+        <is>
+          <t>Eating Out</t>
+        </is>
+      </c>
+      <c r="N1259" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" s="1" t="inlineStr">
+        <is>
+          <t>dbf2acb1-e32c-4dd3-a630-7f10d91f6f15</t>
+        </is>
+      </c>
+      <c r="B1260" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1260" s="2" t="n">
+        <v>44990</v>
+      </c>
+      <c r="D1260" s="2" t="n">
+        <v>44981</v>
+      </c>
+      <c r="E1260" s="2" t="n">
+        <v>44983</v>
+      </c>
+      <c r="F1260" t="inlineStr">
+        <is>
+          <t>SQ *BARISTA</t>
+        </is>
+      </c>
+      <c r="G1260" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1260" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1260" t="n">
+        <v>-15.25</v>
+      </c>
+      <c r="J1260" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1260" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1260" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1260" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="N1260" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" s="1" t="inlineStr">
+        <is>
+          <t>d73b2b92-fde4-4a73-bd17-afa776a9e857</t>
+        </is>
+      </c>
+      <c r="B1261" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1261" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1261" s="2" t="n">
+        <v>44982</v>
+      </c>
+      <c r="E1261" s="2" t="n">
+        <v>44983</v>
+      </c>
+      <c r="F1261" t="inlineStr">
+        <is>
+          <t>SQ *BARISTA</t>
+        </is>
+      </c>
+      <c r="G1261" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1261" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1261" t="n">
+        <v>-12.9</v>
+      </c>
+      <c r="J1261" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1261" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1261" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1261" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="N1261" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" s="1" t="inlineStr">
+        <is>
+          <t>c200d297-987c-4a7c-9f11-8818bfe4c905</t>
+        </is>
+      </c>
+      <c r="B1262" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1262" s="2" t="n">
+        <v>44990</v>
+      </c>
+      <c r="D1262" s="2" t="n">
+        <v>44980</v>
+      </c>
+      <c r="E1262" s="2" t="n">
+        <v>44983</v>
+      </c>
+      <c r="F1262" t="inlineStr">
+        <is>
+          <t>TST* The Fireside</t>
+        </is>
+      </c>
+      <c r="G1262" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1262" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1262" t="n">
+        <v>-35</v>
+      </c>
+      <c r="J1262" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1262" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1262" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1262" t="inlineStr">
+        <is>
+          <t>Eating Out</t>
+        </is>
+      </c>
+      <c r="N1262" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" s="1" t="inlineStr">
+        <is>
+          <t>4162d5d9-88e3-46f2-b529-e02d2a3d8d04</t>
+        </is>
+      </c>
+      <c r="B1263" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1263" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1263" s="2" t="n">
+        <v>44980</v>
+      </c>
+      <c r="E1263" s="2" t="n">
+        <v>44981</v>
+      </c>
+      <c r="F1263" t="inlineStr">
+        <is>
+          <t>SQ *THE DRAGONFLY COFFEE</t>
+        </is>
+      </c>
+      <c r="G1263" t="inlineStr">
+        <is>
+          <t>Food &amp; Drink</t>
+        </is>
+      </c>
+      <c r="H1263" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1263" t="n">
+        <v>-7.25</v>
+      </c>
+      <c r="J1263" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1263" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1263" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1263" t="inlineStr">
+        <is>
+          <t>Coffee</t>
+        </is>
+      </c>
+      <c r="N1263" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" s="1" t="inlineStr">
+        <is>
+          <t>01b6d919-a4e2-4e58-b0d6-417d13c79c5d</t>
+        </is>
+      </c>
+      <c r="B1264" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1264" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1264" s="2" t="n">
+        <v>44978</v>
+      </c>
+      <c r="E1264" s="2" t="n">
+        <v>44979</v>
+      </c>
+      <c r="F1264" t="inlineStr">
+        <is>
+          <t>TRADER JOE'S #146  QPS</t>
+        </is>
+      </c>
+      <c r="G1264" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="H1264" t="inlineStr">
+        <is>
+          <t>Sale</t>
+        </is>
+      </c>
+      <c r="I1264" t="n">
+        <v>-84.34999999999999</v>
+      </c>
+      <c r="J1264" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1264" t="inlineStr">
+        <is>
+          <t>Sapphire</t>
+        </is>
+      </c>
+      <c r="L1264" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1264" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="N1264" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" s="1" t="inlineStr">
+        <is>
+          <t>c46c0b49-2fbd-4338-a299-c82e7966e8fb</t>
+        </is>
+      </c>
+      <c r="B1265" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1265" t="inlineStr"/>
+      <c r="D1265" s="2" t="n">
+        <v>44978</v>
+      </c>
+      <c r="E1265" t="inlineStr"/>
+      <c r="F1265" t="inlineStr">
+        <is>
+          <t>CHASE CREDIT CRD AUTOPAY 000000000582661</t>
+        </is>
+      </c>
+      <c r="G1265" t="inlineStr"/>
+      <c r="H1265" t="inlineStr"/>
+      <c r="I1265" t="n">
+        <v>-1074.39</v>
+      </c>
+      <c r="J1265" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1265" t="inlineStr">
+        <is>
+          <t>Mechanics</t>
+        </is>
+      </c>
+      <c r="L1265" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1265" t="inlineStr"/>
+      <c r="N1265" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" s="1" t="inlineStr">
+        <is>
+          <t>5c206ce6-cbd3-45fb-ac3c-c67331ce3292</t>
+        </is>
+      </c>
+      <c r="B1266" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="C1266" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="D1266" s="2" t="n">
+        <v>44974</v>
+      </c>
+      <c r="E1266" t="inlineStr"/>
+      <c r="F1266" t="inlineStr">
+        <is>
+          <t>TOYOTA MOTOR SAL PAYROLL 568349-TLS</t>
+        </is>
+      </c>
+      <c r="G1266" t="inlineStr"/>
+      <c r="H1266" t="inlineStr"/>
+      <c r="I1266" t="n">
+        <v>1830.19</v>
+      </c>
+      <c r="J1266" s="2" t="n">
+        <v>44989</v>
+      </c>
+      <c r="K1266" t="inlineStr">
+        <is>
+          <t>Mechanics</t>
+        </is>
+      </c>
+      <c r="L1266" t="n">
+        <v>1</v>
+      </c>
+      <c r="M1266" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="N1266" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>